<commit_message>
Finished the attribute normalization and prioritization. Still need to do the row summing and the architecture creation
</commit_message>
<xml_diff>
--- a/workbooks/PlatformDatabase2.xlsx
+++ b/workbooks/PlatformDatabase2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Platform" sheetId="4" r:id="rId1"/>
@@ -693,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1242,8 +1242,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1302,7 @@
         <v>48</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>